<commit_message>
Compare admittance spectrum of GFM and GFL
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/SingleApparatusInfiniteBus/GflInverterInfiniteBus.xlsx
+++ b/Examples/AcPowerSystem/SingleApparatusInfiniteBus/GflInverterInfiniteBus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\SingleApparatusInfiniteBus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C331B8-60BC-4C8E-94AF-DC61FCD14D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0BFA0F-9177-4CA2-8BAB-CC842C51E76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,8 +262,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>inf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Vdc (pu)</t>
+  </si>
+  <si>
+    <t>Cdc (pu)</t>
+  </si>
+  <si>
+    <t>wL (pu)</t>
+  </si>
+  <si>
+    <t>R (pu)</t>
+  </si>
+  <si>
+    <t>BW vdc (Hz)</t>
+  </si>
+  <si>
+    <t>BW PLL (Hz)</t>
+  </si>
+  <si>
+    <t>BW idq (Hz)</t>
   </si>
 </sst>
 </file>
@@ -762,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -792,58 +809,83 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="3"/>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>90</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>2.5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>1.25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>0.05</v>
       </c>
-      <c r="F5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F6" s="2">
+        <f>E6/10</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="2">
         <v>10</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H6" s="2">
         <v>10</v>
       </c>
-      <c r="I5" s="2">
-        <v>250</v>
+      <c r="I6" s="2">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +982,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1024,11 +1066,11 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <f>D11/5</f>
-        <v>0.06</v>
+        <f>D11/10</f>
+        <v>0.01</v>
       </c>
       <c r="D11">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1041,27 +1083,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1141,7 +1163,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1204,7 +1226,7 @@
         <v>39</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
State space model final
Rename files.

The state space models of both GFM and GFL inverters have been tested and compared with toolbox: The swing-frame-based analysis coincide with toolbox properly. But the steady-frame-based analysis still have some little and unknown errors.
</commit_message>
<xml_diff>
--- a/Examples/AcPowerSystem/SingleApparatusInfiniteBus/GflInverterInfiniteBus.xlsx
+++ b/Examples/AcPowerSystem/SingleApparatusInfiniteBus/GflInverterInfiniteBus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\AcPowerSystem\SingleApparatusInfiniteBus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C331B8-60BC-4C8E-94AF-DC61FCD14D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD1541-24DA-4203-80BB-48BAE73A4136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="915" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,7 +624,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -732,7 +732,7 @@
         <v>0.5</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="2">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1204,7 +1204,7 @@
         <v>39</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>